<commit_message>
Avaliações AV Wyden UniRuy 2025.2 - 01122025
</commit_message>
<xml_diff>
--- a/AVA Segundo Sem Wyden UniRuy - 2025_2/Turma Sistemas Operacionais - 3001 Wyden UniRuy 2025_2.xlsx
+++ b/AVA Segundo Sem Wyden UniRuy - 2025_2/Turma Sistemas Operacionais - 3001 Wyden UniRuy 2025_2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\heleno\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9EEF1A1-8531-4291-9F80-0C26874F9A85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E810BA60-E145-426D-93DA-D7C237106869}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{DD6ED3E7-57DF-4A52-9E4C-63B0F7661B3D}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="36">
   <si>
     <t>ALUNO</t>
   </si>
@@ -110,18 +110,6 @@
     <t>https://github.com/Deusyth/Sistema-Operacional</t>
   </si>
   <si>
-    <t>Google Drive bloqueado https://drive.google.com/drive/folders/1VP3zNeLiFA3whe1aasCL263IKJG56CJB?usp=drive_link</t>
-  </si>
-  <si>
-    <t>https://github.com/typeapositive/VM_AtividadeGiovannaAlmeida</t>
-  </si>
-  <si>
-    <t>https://github.com/LuffyBaiano27/Maquina-Virtual</t>
-  </si>
-  <si>
-    <t>https://github.com/almeidaprog/AtividadeVM-Heleno</t>
-  </si>
-  <si>
     <t>https://github.com/trabucoo/AtividadeSO-1</t>
   </si>
   <si>
@@ -132,6 +120,30 @@
   </si>
   <si>
     <t>NÃO</t>
+  </si>
+  <si>
+    <t>AP</t>
+  </si>
+  <si>
+    <t>https://github.com/Christian-Oli/TrabalhoSO-1---VM-; https://github.com/Christian-Oli/TrabalhoSO-4---Pol-tica-de-Seguran-a/blob/main/Trabalho_SO%5B1%5D%20(1).docx</t>
+  </si>
+  <si>
+    <t>MD</t>
+  </si>
+  <si>
+    <t>https://github.com/GabriellaMizrach/Atividade-04-Academica-Politica-de-Seguranca-no-Windows</t>
+  </si>
+  <si>
+    <t>https://github.com/LuffyBaiano27/Maquina-Virtual; https://github.com/LuffyBaiano27/Trabalho-SO-comando-em-modo-Shell</t>
+  </si>
+  <si>
+    <t>https://github.com/typeapositive/VM_AtividadeGiovannaAlmeida;https://github.com/typeapositive?tab=repositories</t>
+  </si>
+  <si>
+    <t>https://github.com/almeidaprog/AtividadeVM-Heleno; https://github.com/almeidaprog/DOS-CMD-HELENO-2025/tree/main</t>
+  </si>
+  <si>
+    <t>https://github.com/TaiLeite/Trabalho-de-SO---Maquina-Virtual</t>
   </si>
 </sst>
 </file>
@@ -167,7 +179,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -186,8 +198,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -324,11 +348,69 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -346,11 +428,42 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -686,316 +799,429 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0212B8F-44EC-4B38-84EB-21D2846DA7CB}">
   <sheetPr codeName="Planilha1"/>
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="78.85546875" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="4" width="5" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="4.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="4"/>
+    <col min="5" max="6" width="4.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="4.5703125" style="4" customWidth="1"/>
+    <col min="8" max="8" width="16.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="24" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="H1" s="5" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="22">
+        <v>2</v>
+      </c>
+      <c r="C2" s="22">
+        <v>2</v>
+      </c>
+      <c r="D2" s="22">
+        <v>2</v>
+      </c>
+      <c r="E2" s="22">
+        <v>1</v>
+      </c>
+      <c r="F2" s="23">
+        <v>2</v>
+      </c>
+      <c r="G2" s="11">
+        <f>SUM(B2:F2)</f>
+        <v>9</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="15">
+        <v>2</v>
+      </c>
+      <c r="C3" s="15">
+        <v>2</v>
+      </c>
+      <c r="D3" s="15">
+        <v>2</v>
+      </c>
+      <c r="E3" s="15">
+        <v>1</v>
+      </c>
+      <c r="F3" s="16">
+        <v>0</v>
+      </c>
+      <c r="G3" s="19">
+        <f t="shared" ref="G3:G15" si="0">SUM(B3:F3)</f>
+        <v>7</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="15">
+        <v>1</v>
+      </c>
+      <c r="C4" s="15">
+        <v>1</v>
+      </c>
+      <c r="D4" s="15">
+        <v>1</v>
+      </c>
+      <c r="E4" s="15">
+        <v>1</v>
+      </c>
+      <c r="F4" s="16">
+        <v>2</v>
+      </c>
+      <c r="G4" s="19">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C5" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D5" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="E5" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F5" s="18">
+        <v>0</v>
+      </c>
+      <c r="G5" s="25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H5" s="26" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="22">
+        <v>2</v>
+      </c>
+      <c r="C6" s="22">
+        <v>2</v>
+      </c>
+      <c r="D6" s="22">
+        <v>2</v>
+      </c>
+      <c r="E6" s="22">
+        <v>2</v>
+      </c>
+      <c r="F6" s="23">
+        <v>2</v>
+      </c>
+      <c r="G6" s="19">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="H6" s="4" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="11" t="s">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="22">
+        <v>2</v>
+      </c>
+      <c r="C7" s="22">
+        <v>2</v>
+      </c>
+      <c r="D7" s="22">
+        <v>2</v>
+      </c>
+      <c r="E7" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="F7" s="16">
+        <v>2</v>
+      </c>
+      <c r="G7" s="19">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="15">
+        <v>2</v>
+      </c>
+      <c r="C8" s="15">
+        <v>2</v>
+      </c>
+      <c r="D8" s="15">
+        <v>2</v>
+      </c>
+      <c r="E8" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="F8" s="16">
+        <v>2</v>
+      </c>
+      <c r="G8" s="19">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="15">
+        <v>2</v>
+      </c>
+      <c r="C9" s="15">
+        <v>2</v>
+      </c>
+      <c r="D9" s="15">
+        <v>2</v>
+      </c>
+      <c r="E9" s="15">
+        <v>1</v>
+      </c>
+      <c r="F9" s="16">
+        <v>2</v>
+      </c>
+      <c r="G9" s="19">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="15">
+        <v>2</v>
+      </c>
+      <c r="C10" s="15">
+        <v>2</v>
+      </c>
+      <c r="D10" s="15">
+        <v>2</v>
+      </c>
+      <c r="E10" s="15">
+        <v>1</v>
+      </c>
+      <c r="F10" s="16">
+        <v>2</v>
+      </c>
+      <c r="G10" s="19">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="15">
+        <v>2</v>
+      </c>
+      <c r="C11" s="15">
+        <v>2</v>
+      </c>
+      <c r="D11" s="15">
+        <v>2</v>
+      </c>
+      <c r="E11" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="11" t="s">
+      <c r="F11" s="16">
+        <v>2</v>
+      </c>
+      <c r="G11" s="19">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="11" t="s">
+      <c r="C12" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="D12" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="11" t="s">
+      <c r="E12" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="11" t="s">
+      <c r="F12" s="18">
+        <v>0</v>
+      </c>
+      <c r="G12" s="25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H12" s="26" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="15">
+        <v>2</v>
+      </c>
+      <c r="C13" s="15">
+        <v>2</v>
+      </c>
+      <c r="D13" s="15">
+        <v>2</v>
+      </c>
+      <c r="E13" s="15">
+        <v>1</v>
+      </c>
+      <c r="F13" s="16">
+        <v>2</v>
+      </c>
+      <c r="G13" s="19">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" s="15">
+        <v>0.5</v>
+      </c>
+      <c r="C14" s="15">
+        <v>1.5</v>
+      </c>
+      <c r="D14" s="15">
+        <v>1.5</v>
+      </c>
+      <c r="E14" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="7" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="E5" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="F5" s="7" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="E6" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="D7" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="E7" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="E8" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="C9" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="D9" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="E9" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="C10" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="D10" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="E10" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="F10" s="4" t="s">
+      <c r="F14" s="16">
+        <v>2</v>
+      </c>
+      <c r="G14" s="19">
+        <f t="shared" si="0"/>
+        <v>5.5</v>
+      </c>
+      <c r="H14" s="7" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="B11" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="C11" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="D11" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="E11" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="B12" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="C12" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="D12" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="E12" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="F12" s="7" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="B13" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="C13" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="D13" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="E13" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="F13" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="B14" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="C14" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="D14" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="E14" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="F14" s="7" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B15" s="12"/>
-      <c r="C15" s="12"/>
-      <c r="D15" s="12"/>
-      <c r="E15" s="12"/>
-      <c r="F15" s="7" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B15" s="20">
+        <v>2</v>
+      </c>
+      <c r="C15" s="20">
+        <v>1.5</v>
+      </c>
+      <c r="D15" s="20">
+        <v>1.5</v>
+      </c>
+      <c r="E15" s="20">
+        <v>1</v>
+      </c>
+      <c r="F15" s="21">
+        <v>2</v>
+      </c>
+      <c r="G15" s="12">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="H15" s="7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
         <v>3</v>
       </c>

</xml_diff>